<commit_message>
Se suben ultimos cambios respecto al json
</commit_message>
<xml_diff>
--- a/src/test/resources/data/excel/test_data.xlsx
+++ b/src/test/resources/data/excel/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Orlando\Desktop\TSOFT\PROYECTOS\Mi Banco\FrameWork Servicios\mibanco_auto_api\src\test\resources\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C0642B-59DE-4062-8FA3-47C3D3905DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62BD6AC-A493-4452-B010-C2B51B9F46D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D67BDC7E-500E-42C9-AB4D-08B688548481}"/>
   </bookViews>
@@ -108,11 +108,11 @@
     <t>token</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>{
     "email": "eve.holt@reqres.in"}</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="3" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>19</v>
@@ -639,7 +639,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="4">
         <v>400</v>
@@ -650,7 +650,7 @@
     </row>
     <row r="4" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>12</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Se sube reporte html
</commit_message>
<xml_diff>
--- a/src/test/resources/data/excel/test_data.xlsx
+++ b/src/test/resources/data/excel/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Orlando\Desktop\TSOFT\PROYECTOS\Mi Banco\FrameWork Servicios\mibanco_auto_api\src\test\resources\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62BD6AC-A493-4452-B010-C2B51B9F46D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37085398-4046-4E83-9E2F-DA128EF16317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D67BDC7E-500E-42C9-AB4D-08B688548481}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Endpoint</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Expected Status Code</t>
   </si>
   <si>
-    <t>Expected Content</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
   </si>
   <si>
     <t>PUT</t>
-  </si>
-  <si>
-    <t>{"status": "ok"}</t>
   </si>
   <si>
     <t>https://jsonplaceholder.typicode.com/todos/1</t>
@@ -93,9 +87,6 @@
     <t>Authorization: Bearer my_token</t>
   </si>
   <si>
-    <t>{"success": true}</t>
-  </si>
-  <si>
     <t>https://reqres.in/api/login</t>
   </si>
   <si>
@@ -113,6 +104,40 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Expected Content_2</t>
+  </si>
+  <si>
+    <t>Expected Content_3</t>
+  </si>
+  <si>
+    <t>Expected Content_4</t>
+  </si>
+  <si>
+    <t>Expected Content_5</t>
+  </si>
+  <si>
+    <t>Expected Content_6</t>
+  </si>
+  <si>
+    <t>Expected Content_1</t>
+  </si>
+  <si>
+    <t>{"id":1}</t>
+  </si>
+  <si>
+    <t>{
+    "id": 1
+}</t>
+  </si>
+  <si>
+    <t>{
+    "error": "Missing password"
+}</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -567,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A00CB2-873E-43C5-83B7-E9868A7B8F5C}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,12 +605,13 @@
     <col min="4" max="4" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="12" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -597,121 +623,165 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4">
         <v>200</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4">
         <v>400</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="4">
         <v>201</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4">
         <v>200</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4">
         <v>201</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="6"/>
       <c r="C7" s="4"/>
@@ -719,8 +789,13 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="6"/>
       <c r="C8" s="4"/>
@@ -728,8 +803,13 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
@@ -737,8 +817,13 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
@@ -746,8 +831,13 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
@@ -755,8 +845,13 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
@@ -764,8 +859,13 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
@@ -773,8 +873,13 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
@@ -782,8 +887,13 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
@@ -791,8 +901,13 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="4"/>
@@ -800,8 +915,13 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
@@ -809,8 +929,13 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
@@ -818,8 +943,13 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="4"/>
@@ -827,8 +957,13 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="4"/>
@@ -836,8 +971,13 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="6"/>
       <c r="C21" s="4"/>
@@ -845,8 +985,13 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="4"/>
@@ -854,8 +999,13 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="6"/>
       <c r="C23" s="4"/>
@@ -863,8 +1013,13 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
       <c r="C24" s="4"/>
@@ -872,8 +1027,13 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="6"/>
       <c r="C25" s="4"/>
@@ -881,8 +1041,13 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="6"/>
       <c r="C26" s="4"/>
@@ -890,8 +1055,13 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="6"/>
       <c r="C27" s="4"/>
@@ -899,8 +1069,13 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="6"/>
       <c r="C28" s="4"/>
@@ -908,8 +1083,13 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="6"/>
       <c r="C29" s="4"/>
@@ -917,8 +1097,13 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
       <c r="C30" s="4"/>
@@ -926,8 +1111,13 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="6"/>
       <c r="C31" s="4"/>
@@ -935,8 +1125,13 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="6"/>
       <c r="C32" s="4"/>
@@ -944,8 +1139,13 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="6"/>
       <c r="C33" s="4"/>
@@ -953,8 +1153,13 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="6"/>
       <c r="C34" s="4"/>
@@ -962,8 +1167,13 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
@@ -971,8 +1181,13 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="6"/>
       <c r="C36" s="4"/>
@@ -980,8 +1195,13 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="6"/>
       <c r="C37" s="4"/>
@@ -989,8 +1209,13 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="6"/>
       <c r="C38" s="4"/>
@@ -998,8 +1223,13 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="6"/>
       <c r="C39" s="4"/>
@@ -1007,8 +1237,13 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="6"/>
       <c r="C40" s="4"/>
@@ -1016,8 +1251,13 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="6"/>
       <c r="C41" s="4"/>
@@ -1025,8 +1265,13 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="5"/>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="6"/>
       <c r="C42" s="4"/>
@@ -1034,8 +1279,13 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="6"/>
       <c r="C43" s="4"/>
@@ -1043,8 +1293,13 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="6"/>
       <c r="C44" s="4"/>
@@ -1052,8 +1307,13 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="6"/>
       <c r="C45" s="4"/>
@@ -1061,8 +1321,13 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="6"/>
       <c r="C46" s="4"/>
@@ -1070,6 +1335,11 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>